<commit_message>
Changed database scheme. Added adding and changing route lists.
</commit_message>
<xml_diff>
--- a/Data/Пример маршрутного листа.xlsx
+++ b/Data/Пример маршрутного листа.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\RouteLists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ReZuCoS\Programming files\RouteLists\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE80E155-C31A-4DDE-BEAB-C53C4EA2A83D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486F4D86-3422-4439-A107-AC0280CA0D1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,12 +196,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -240,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -270,26 +276,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -571,9 +583,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -589,17 +601,17 @@
     <col min="8" max="8" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -607,17 +619,17 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -625,17 +637,17 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -643,17 +655,17 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -661,17 +673,17 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -679,23 +691,23 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="18" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -704,12 +716,20 @@
       <c r="H6" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+    </row>
+    <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -726,12 +746,20 @@
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+    </row>
+    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>2</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -749,11 +777,11 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>3</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -771,11 +799,11 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>4</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -793,11 +821,11 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>5</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -815,11 +843,11 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>6</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -837,11 +865,11 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>7</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -859,11 +887,11 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>8</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -881,21 +909,21 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11" t="s">
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
@@ -907,14 +935,14 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>40</v>
       </c>
       <c r="D17" s="14"/>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="12" t="s">
         <v>37</v>
       </c>
       <c r="F17" s="14" t="s">
@@ -925,17 +953,17 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="11" t="s">
         <v>38</v>
       </c>
       <c r="D18" s="10"/>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="11" t="s">
         <v>38</v>
       </c>
       <c r="G18" s="8"/>
@@ -952,18 +980,18 @@
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16" t="s">
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
@@ -977,14 +1005,14 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>41</v>
       </c>
       <c r="D22" s="14"/>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="12" t="s">
         <v>37</v>
       </c>
       <c r="F22" s="14" t="s">
@@ -995,17 +1023,17 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="11" t="s">
         <v>38</v>
       </c>
       <c r="D23" s="8"/>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="11" t="s">
         <v>38</v>
       </c>
       <c r="G23" s="10"/>

</xml_diff>

<commit_message>
[Version 1] Updated database structure, code refactorings, added settings menu, route lists to excel export.
</commit_message>
<xml_diff>
--- a/Data/Пример маршрутного листа.xlsx
+++ b/Data/Пример маршрутного листа.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ReZuCoS\Programming files\RouteLists\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486F4D86-3422-4439-A107-AC0280CA0D1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948054DB-0A3A-47B6-9117-AB42DCA97EBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
   <si>
     <t>Маршрутный лист № МЛ-Е285УО799-01042022</t>
   </si>
@@ -168,6 +168,15 @@
   </si>
   <si>
     <t>Филимонов Ф. Ф., Водитель</t>
+  </si>
+  <si>
+    <t>Маршрутный лист выдан "___" ________  2022 г. в __ ч __ мин</t>
+  </si>
+  <si>
+    <t>_____________/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           (Ф.И.О., должность)</t>
   </si>
 </sst>
 </file>
@@ -246,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -285,23 +294,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,15 +597,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" style="5" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
@@ -602,16 +614,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -620,16 +632,16 @@
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -638,16 +650,16 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -656,16 +668,16 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -674,16 +686,16 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -695,19 +707,19 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="14" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -716,16 +728,16 @@
       <c r="H6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-    </row>
-    <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+    </row>
+    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -746,16 +758,16 @@
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-    </row>
-    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>2</v>
       </c>
@@ -777,7 +789,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>3</v>
       </c>
@@ -799,7 +811,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>4</v>
       </c>
@@ -821,7 +833,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>5</v>
       </c>
@@ -843,7 +855,7 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>6</v>
       </c>
@@ -887,7 +899,7 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>8</v>
       </c>
@@ -910,18 +922,18 @@
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
@@ -938,17 +950,17 @@
       <c r="B17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="14"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="14"/>
+      <c r="G17" s="16"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -956,8 +968,8 @@
       <c r="B18" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>38</v>
+      <c r="C18" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="11" t="s">
@@ -980,18 +992,18 @@
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17" t="s">
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
@@ -1008,17 +1020,17 @@
       <c r="B22" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="14"/>
+      <c r="D22" s="16"/>
       <c r="E22" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="14"/>
+      <c r="G22" s="16"/>
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1055,7 +1067,7 @@
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A2:H2"/>
   </mergeCells>
-  <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="1.1811023622047245" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>